<commit_message>
Fixed excerpt in Applications Report
</commit_message>
<xml_diff>
--- a/Briefing Note Enrolment Comparison Table From Previous Academic Year.xlsx
+++ b/Briefing Note Enrolment Comparison Table From Previous Academic Year.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://keyanomailca-my.sharepoint.com/personal/bill_guo_keyano_ca/Documents/Documents/KPI-Automation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://keyanomailca-my.sharepoint.com/personal/bill_guo_keyano_ca/Documents/Documents/KPI-Automation-Final-Products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{125920BB-BE59-4A23-8F35-B4780568970F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87DA442C-41FD-458D-9EBF-F0D72B5A810D}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{125920BB-BE59-4A23-8F35-B4780568970F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD289AA9-2B1B-42F4-B4FE-EE59FA0065E1}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C89FB34-6A01-4E4F-A7F7-02F8C0983CC0}"/>
   </bookViews>
@@ -107,7 +107,7 @@
     <t>***No need to fill in grey cells***</t>
   </si>
   <si>
-    <t>2024-06-10 (2024-25)</t>
+    <t>2024-08-01 (2024-25)</t>
   </si>
 </sst>
 </file>
@@ -408,6 +408,18 @@
     <xf numFmtId="10" fontId="7" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -490,18 +502,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -841,7 +841,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,51 +862,51 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="33" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="40" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="37"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="41"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="24"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
@@ -919,22 +919,22 @@
       <c r="F5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="35"/>
-      <c r="H5" s="38"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="42"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="39">
-        <v>2040</v>
-      </c>
-      <c r="D6" s="40">
-        <v>1167.6690000000001</v>
+      <c r="C6" s="11">
+        <v>2680</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1614.873</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -943,15 +943,15 @@
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="41">
-        <v>1286</v>
-      </c>
-      <c r="D7" s="42">
-        <v>789.07799999999997</v>
+      <c r="C7" s="13">
+        <v>1540</v>
+      </c>
+      <c r="D7" s="14">
+        <v>997.14599999999996</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="7"/>
@@ -960,15 +960,15 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="41">
-        <v>754</v>
-      </c>
-      <c r="D8" s="42">
-        <v>378.59100000000001</v>
+      <c r="C8" s="13">
+        <v>1140</v>
+      </c>
+      <c r="D8" s="14">
+        <v>617.72699999999998</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -977,15 +977,15 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="41">
-        <v>42</v>
-      </c>
-      <c r="D9" s="42">
-        <v>14.318</v>
+      <c r="C9" s="13">
+        <v>77</v>
+      </c>
+      <c r="D9" s="14">
+        <v>27.352</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -994,15 +994,15 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="41">
-        <v>260</v>
-      </c>
-      <c r="D10" s="42">
-        <v>73.147000000000006</v>
+      <c r="C10" s="13">
+        <v>355</v>
+      </c>
+      <c r="D10" s="14">
+        <v>96.382000000000005</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -1011,17 +1011,17 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="41">
-        <v>560</v>
-      </c>
-      <c r="D11" s="42">
-        <v>206.82</v>
+      <c r="C11" s="13">
+        <v>780</v>
+      </c>
+      <c r="D11" s="14">
+        <v>305.15499999999997</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1030,15 +1030,15 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="41">
-        <v>1269</v>
-      </c>
-      <c r="D12" s="42">
-        <v>788.58199999999999</v>
+      <c r="C12" s="13">
+        <v>1573</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1031.5119999999999</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -1047,15 +1047,15 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="41">
-        <v>226</v>
-      </c>
-      <c r="D13" s="42">
-        <v>172.267</v>
+      <c r="C13" s="13">
+        <v>352</v>
+      </c>
+      <c r="D13" s="14">
+        <v>275.20600000000002</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -1064,17 +1064,17 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="18" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="41">
-        <v>1675</v>
-      </c>
-      <c r="D14" s="42">
-        <v>750.827</v>
+      <c r="C14" s="13">
+        <v>2288</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1029.1020000000001</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -1083,15 +1083,15 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="41">
-        <v>533</v>
-      </c>
-      <c r="D15" s="42">
-        <v>224.136</v>
+      <c r="C15" s="13">
+        <v>898</v>
+      </c>
+      <c r="D15" s="14">
+        <v>378.79700000000003</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>

</xml_diff>